<commit_message>
recreated routing with better ground plane
</commit_message>
<xml_diff>
--- a/pin-analysis.xlsx
+++ b/pin-analysis.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="82">
   <si>
     <t xml:space="preserve">pin</t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">port</t>
   </si>
   <si>
+    <t xml:space="preserve">power domain</t>
+  </si>
+  <si>
     <t xml:space="preserve">Analog</t>
   </si>
   <si>
@@ -46,79 +49,82 @@
     <t xml:space="preserve">XTAL</t>
   </si>
   <si>
+    <t xml:space="preserve">VDDANA</t>
+  </si>
+  <si>
     <t xml:space="preserve">PA02</t>
   </si>
   <si>
     <t xml:space="preserve">AIN0</t>
   </si>
   <si>
+    <t xml:space="preserve">D3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AIN1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AIN4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2_DFM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AIN5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1_DTM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AIN6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-2</t>
+  </si>
+  <si>
     <t xml:space="preserve">A1</t>
   </si>
   <si>
-    <t xml:space="preserve">PA03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AIN1</t>
+    <t xml:space="preserve">PA07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AIN7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-3</t>
   </si>
   <si>
     <t xml:space="preserve">A2</t>
   </si>
   <si>
-    <t xml:space="preserve">PA04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AIN4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D2_DFM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PA05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AIN5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D1_DTM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PA06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AIN6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D3_INT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PA07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AIN7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D4_INT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VDDANA</t>
-  </si>
-  <si>
     <t xml:space="preserve">GND</t>
   </si>
   <si>
     <t xml:space="preserve">PA08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VDDIO</t>
   </si>
   <si>
     <t xml:space="preserve">AIN16</t>
@@ -275,6 +281,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -349,11 +356,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -434,17 +441,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -469,13 +476,19 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -483,22 +496,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>10</v>
+      <c r="D4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -506,13 +525,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="0" t="s">
         <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -520,16 +542,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>17</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -537,16 +562,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>21</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -554,19 +582,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="G8" s="0" t="s">
-        <v>25</v>
+      <c r="H8" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -574,52 +605,63 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="G9" s="0" t="s">
-        <v>29</v>
-      </c>
+      <c r="H9" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>31</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>11</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="0" t="s">
         <v>33</v>
       </c>
+      <c r="C13" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="D13" s="0" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>34</v>
+        <v>18</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -627,16 +669,19 @@
         <v>12</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>37</v>
+        <v>22</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -644,16 +689,19 @@
         <v>13</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>40</v>
+        <v>26</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -661,16 +709,19 @@
         <v>14</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>43</v>
+        <v>30</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -678,13 +729,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>40</v>
+        <v>46</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -692,13 +746,21 @@
         <v>16</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -706,16 +768,19 @@
         <v>17</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="G20" s="0" t="s">
         <v>51</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -723,16 +788,19 @@
         <v>18</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="G21" s="0" t="s">
+      <c r="C21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>55</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -740,13 +808,16 @@
         <v>19</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -754,13 +825,16 @@
         <v>20</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -768,13 +842,16 @@
         <v>21</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -782,13 +859,16 @@
         <v>22</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H25" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -796,13 +876,16 @@
         <v>23</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="H26" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -810,13 +893,21 @@
         <v>24</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="H27" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -824,10 +915,13 @@
         <v>25</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="H29" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -835,15 +929,19 @@
         <v>26</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>72</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="C30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="n">
+      <c r="A31" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>73</v>
+      <c r="B31" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -851,56 +949,76 @@
         <v>28</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>31</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
         <v>29</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>74</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="C33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
         <v>30</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>75</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="C34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
         <v>31</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>76</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="C35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
         <v>32</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>77</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C41" s="2"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
         <v>0</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="F42" s="0" t="s">
-        <v>63</v>
+        <v>80</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -908,19 +1026,19 @@
         <v>1</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E43" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="G43" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="H43" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="F43" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="G43" s="0" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -928,30 +1046,30 @@
         <v>2</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="G44" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="H44" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E45" s="0" t="s">
+      <c r="F45" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="G45" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="H45" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="F45" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="G45" s="0" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>